<commit_message>
rHub, Piao, Qinchui Stage Almost finish.
</commit_message>
<xml_diff>
--- a/i wanna play with Mr. Zombie/进度一览.xlsx
+++ b/i wanna play with Mr. Zombie/进度一览.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\i-wanna\i wanna play with Mr. Zombie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4709B251-CC1C-443C-966B-F7A14A916D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F45B7C-9C08-4E03-9A66-BD22202E2040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26914B40-D71E-42E6-873D-934C67124CCD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
   <si>
     <t>BGM</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -436,38 +436,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>已完工（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>GM8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
         <family val="2"/>
         <charset val="134"/>
       </rPr>
@@ -481,32 +449,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>需要重新发一下</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>未知</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
         <family val="2"/>
         <charset val="134"/>
       </rPr>
@@ -649,27 +591,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>退潮、</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>sparkshadow</t>
-    </r>
+    <t>已完工</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已整合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -677,7 +615,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -734,13 +672,27 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -757,7 +709,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -768,9 +720,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1090,7 +1057,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1130,11 +1097,11 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>24</v>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>25</v>
@@ -1221,11 +1188,23 @@
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
@@ -1247,7 +1226,7 @@
       <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1264,22 +1243,34 @@
       <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>24</v>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1291,60 +1282,75 @@
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="F11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>33</v>
+      <c r="B12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>34</v>
+      <c r="C14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="E15" s="7"/>
       <c r="F15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
@@ -1352,15 +1358,15 @@
     </row>
     <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>20</v>
@@ -1368,18 +1374,18 @@
     </row>
     <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish second test, waiting for ED. Add some meme.
</commit_message>
<xml_diff>
--- a/i wanna play with Mr. Zombie/进度一览.xlsx
+++ b/i wanna play with Mr. Zombie/进度一览.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\i-wanna\i wanna play with Mr. Zombie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F96E110-EC17-4A1F-B9FF-96696BE6D7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170D358A-A851-4E0F-854F-F69EBC889D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26914B40-D71E-42E6-873D-934C67124CCD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
   <si>
     <t>BGM</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -469,20 +469,6 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>零梦、猫猫</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
@@ -527,23 +513,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>差无间关卡特效抉择</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>还差削弱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>可能要削</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>测试进度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要改变进入方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小居士</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>因为特效太瞎眼了，所以去掉了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老廖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王者青年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>塞德莎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特特</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>烈焰</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -617,18 +619,12 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -645,7 +641,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -667,20 +663,26 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,23 +998,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5B1E78-E742-4FFC-9800-71ABD77F5DA3}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.796875" style="1"/>
-    <col min="6" max="6" width="17.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.796875" style="1"/>
+    <col min="2" max="2" width="18.296875" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="5" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.296875" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1028,11 +1032,27 @@
       <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="M1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1042,8 +1062,8 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>39</v>
+      <c r="D2" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>26</v>
@@ -1054,42 +1074,47 @@
       <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="G3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="E4" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>24</v>
@@ -1097,11 +1122,9 @@
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1123,11 +1146,9 @@
       <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1150,30 +1171,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1192,11 +1213,14 @@
       <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="H8" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1215,30 +1239,32 @@
       <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1248,44 +1274,48 @@
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="H12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1295,32 +1325,32 @@
       <c r="C14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="12" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
@@ -1328,7 +1358,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1336,34 +1366,26 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="C18" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="G8:G11"/>
     <mergeCell ref="E14:E15"/>
+    <mergeCell ref="H8:H11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>